<commit_message>
Add chart visualization to Excel export
</commit_message>
<xml_diff>
--- a/output_Jaccard.xlsx
+++ b/output_Jaccard.xlsx
@@ -66,8 +66,282 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr anchor="t" rtlCol="false"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="vi-VN"/>
+              <a:t>Runtime &amp; Closed Patterns vs minSup</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="false"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Runtime (ms)</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Results!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7290.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6033.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6184.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5788.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5525.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5279.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="false"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Closed Patterns</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="square"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Results!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Results!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>77242.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69888.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65600.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61157.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55829.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51832.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="false"/>
+        </c:ser>
+        <c:axId val="0"/>
+        <c:axId val="1"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="0"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="false"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr anchor="t" rtlCol="false"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="vi-VN"/>
+                  <a:t>minSup</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="false"/>
+        </c:title>
+        <c:numFmt sourceLinked="true" formatCode=""/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="false"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="false"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr anchor="t" rtlCol="false"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="vi-VN"/>
+                  <a:t>Value</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="false"/>
+        </c:title>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="0"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:overlay val="false"/>
+    </c:legend>
+    <c:plotVisOnly val="true"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name="Diagramm0"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="3733800" cy="3619500"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
@@ -99,7 +373,7 @@
         <v>0.005</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>5922.0</v>
+        <v>7290.0</v>
       </c>
       <c r="C2" t="n" s="0">
         <v>77242.0</v>
@@ -113,7 +387,7 @@
         <v>0.006</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>4963.0</v>
+        <v>6033.0</v>
       </c>
       <c r="C3" t="n" s="0">
         <v>69888.0</v>
@@ -127,7 +401,7 @@
         <v>0.007</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>4838.0</v>
+        <v>6184.0</v>
       </c>
       <c r="C4" t="n" s="0">
         <v>65600.0</v>
@@ -141,7 +415,7 @@
         <v>0.008</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>4608.0</v>
+        <v>5788.0</v>
       </c>
       <c r="C5" t="n" s="0">
         <v>61157.0</v>
@@ -155,7 +429,7 @@
         <v>0.009</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>4407.0</v>
+        <v>5525.0</v>
       </c>
       <c r="C6" t="n" s="0">
         <v>55829.0</v>
@@ -169,7 +443,7 @@
         <v>0.01</v>
       </c>
       <c r="B7" t="n" s="0">
-        <v>5021.0</v>
+        <v>5279.0</v>
       </c>
       <c r="C7" t="n" s="0">
         <v>51832.0</v>
@@ -180,5 +454,6 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>